<commit_message>
Update Config file. Added dev/prod db connections.
</commit_message>
<xml_diff>
--- a/USNRobot_2/Data/Config.xlsx
+++ b/USNRobot_2/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ionut-mihai.nicula\Documents\UiPath\USNRobotDB.1.0.57-alpha.38\lib\net45\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ionut-mihai.nicula\Documents\UiPath\UiPath Projects Assigned\[Internal]USN Robot\Project\USNRobot_2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD552534-AC6F-4F10-B414-ACAC92E04FAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1554EA-6CAD-4FD2-8E40-535030BA85B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="196">
   <si>
     <t>Name</t>
   </si>
@@ -608,6 +608,24 @@
   </si>
   <si>
     <t>USNRobot_RemoteAssessmentCentralizedEmailPassed</t>
+  </si>
+  <si>
+    <t>dbProd</t>
+  </si>
+  <si>
+    <t>Data Source=proj-usn-sql-serv.database.windows.net;Initial Catalog=proj-usn-db;Persist Security Info=True;User ID=bogdan;Password=B3uqzDSy|V4.doY</t>
+  </si>
+  <si>
+    <t>dbDev</t>
+  </si>
+  <si>
+    <t>Data Source=proj-usn-sql-serv.database.windows.net;Initial Catalog=dev-proj-usn;Persist Security Info=True;User ID=bogdan;Password=B3uqzDSy|V4.doY</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>dev</t>
   </si>
 </sst>
 </file>
@@ -1727,10 +1745,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1852,6 +1870,30 @@
         <v>28</v>
       </c>
     </row>
+    <row r="14" spans="1:26">
+      <c r="A14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" t="s">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1862,7 +1904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Process Status 2 Questionare Test failed to send HR Questionnaire again
</commit_message>
<xml_diff>
--- a/USNRobot_2/Data/Config.xlsx
+++ b/USNRobot_2/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ionut-mihai.nicula\Documents\UiPath\UiPath Projects Assigned\[Internal]USN Robot\Project\USNRobot_2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1554EA-6CAD-4FD2-8E40-535030BA85B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAE3324-D4D8-47CE-B9EB-ACD5C34B3D61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="216">
   <si>
     <t>Name</t>
   </si>
@@ -626,6 +626,66 @@
   </si>
   <si>
     <t>dev</t>
+  </si>
+  <si>
+    <t>BioBAPlaceholder</t>
+  </si>
+  <si>
+    <t>USNAddNewCandidate_BioPlacholderBaCandidate</t>
+  </si>
+  <si>
+    <t>BioInfraPlaceholder</t>
+  </si>
+  <si>
+    <t>USNAddNewCandidate_BioPlacholderInfraCandidate</t>
+  </si>
+  <si>
+    <t>BioSaPlaceholder</t>
+  </si>
+  <si>
+    <t>USNAddNewCandidate_BioPlacholderSaCandidate</t>
+  </si>
+  <si>
+    <t>BioDevPlaceholder</t>
+  </si>
+  <si>
+    <t>USNAddNewCandidate_BioPlacholderDevCandidate</t>
+  </si>
+  <si>
+    <t>EmailBioFormBody</t>
+  </si>
+  <si>
+    <t>USNAddNewCandidate_EmailBodyBioForms</t>
+  </si>
+  <si>
+    <t>EmailBioFormSubject</t>
+  </si>
+  <si>
+    <t>USNAddNewCandidate_EmailSubjectBioForms</t>
+  </si>
+  <si>
+    <t>CandidateBioEmailBody</t>
+  </si>
+  <si>
+    <t>USNAddNewCandidate_CandidateBioEmailBody</t>
+  </si>
+  <si>
+    <t>CandidateBioEmailSubject</t>
+  </si>
+  <si>
+    <t>USNAddNewCandidate_CandidateBioEmailSubject</t>
+  </si>
+  <si>
+    <t>CandidateBioFormUrlPlaceholder</t>
+  </si>
+  <si>
+    <t>USNAddNewCandidate_CandidateBioEmail_FormUrlPlaceholder</t>
+  </si>
+  <si>
+    <t>EmailBodyBioPOC</t>
+  </si>
+  <si>
+    <t>USNAddNewCandidate_EmailBodyBioPOC</t>
   </si>
 </sst>
 </file>
@@ -1747,7 +1807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -1902,10 +1962,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1005"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2517,24 +2577,94 @@
         <v>189</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="64" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="63" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A63" t="s">
+        <v>196</v>
+      </c>
+      <c r="B63" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A64" t="s">
+        <v>198</v>
+      </c>
+      <c r="B64" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A65" t="s">
+        <v>200</v>
+      </c>
+      <c r="B65" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A66" t="s">
+        <v>202</v>
+      </c>
+      <c r="B66" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A67" t="s">
+        <v>204</v>
+      </c>
+      <c r="B67" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A68" t="s">
+        <v>206</v>
+      </c>
+      <c r="B68" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A69" t="s">
+        <v>208</v>
+      </c>
+      <c r="B69" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A70" t="s">
+        <v>210</v>
+      </c>
+      <c r="B70" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A71" t="s">
+        <v>212</v>
+      </c>
+      <c r="B71" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A72" t="s">
+        <v>214</v>
+      </c>
+      <c r="B72" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="74" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="76" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="77" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="78" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="79" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="80" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="81" ht="14.25" customHeight="1"/>
     <row r="82" ht="14.25" customHeight="1"/>
     <row r="83" ht="14.25" customHeight="1"/>
@@ -3442,24 +3572,6 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
-    <row r="1002" ht="14.25" customHeight="1"/>
-    <row r="1003" ht="14.25" customHeight="1"/>
-    <row r="1004" ht="14.25" customHeight="1"/>
-    <row r="1005" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
checking score and status of hr test
</commit_message>
<xml_diff>
--- a/USNRobot_2/Data/Config.xlsx
+++ b/USNRobot_2/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ionut-mihai.nicula\Documents\UiPath\UiPath Projects Assigned\[Internal]USN Robot\Project\USNRobot_2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAE3324-D4D8-47CE-B9EB-ACD5C34B3D61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE33336-E3A0-4B9C-BCDA-67A548B95972}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="218">
   <si>
     <t>Name</t>
   </si>
@@ -686,6 +686,12 @@
   </si>
   <si>
     <t>USNAddNewCandidate_EmailBodyBioPOC</t>
+  </si>
+  <si>
+    <t>token</t>
+  </si>
+  <si>
+    <t>Bearer d4ac6a7c3fd658895c1079af45797798553ab84af4f2ea37b39bf32a3f972d79</t>
   </si>
 </sst>
 </file>
@@ -1805,10 +1811,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1954,6 +1960,14 @@
         <v>195</v>
       </c>
     </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>216</v>
+      </c>
+      <c r="B21" t="s">
+        <v>217</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1964,7 +1978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added awaiting for bio
</commit_message>
<xml_diff>
--- a/USNRobot_2/Data/Config.xlsx
+++ b/USNRobot_2/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ionut-mihai.nicula\Documents\UiPath\UiPath Projects Assigned\[Internal]USN Robot\Project\USNRobot_2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE33336-E3A0-4B9C-BCDA-67A548B95972}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B0E61A-5CF8-4ED3-BC5D-5E907E73663C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="248">
   <si>
     <t>Name</t>
   </si>
@@ -692,6 +692,96 @@
   </si>
   <si>
     <t>Bearer d4ac6a7c3fd658895c1079af45797798553ab84af4f2ea37b39bf32a3f972d79</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_baRemoteAssesmentDescription</t>
+  </si>
+  <si>
+    <t>BaRemoteAssesmentDescription</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_baRemoteAssesmentURL</t>
+  </si>
+  <si>
+    <t>BaRemoteAssesmentURL</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_baResults</t>
+  </si>
+  <si>
+    <t>BaResults</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_devRemoteAssesmentDescription</t>
+  </si>
+  <si>
+    <t>DevRemoteAssesmentDescription</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_devRemoteAssesmentURL</t>
+  </si>
+  <si>
+    <t>DevRemoteAssesmentURL</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_devResults</t>
+  </si>
+  <si>
+    <t>DevResults</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_infraRemoteAssesmentDescription</t>
+  </si>
+  <si>
+    <t>InfraRemoteAssesmentDescription</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_infraRemoteAssesmentURL</t>
+  </si>
+  <si>
+    <t>InfraRemoteAssesmentURL</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_infraResults</t>
+  </si>
+  <si>
+    <t>InfraResults</t>
+  </si>
+  <si>
+    <t>SaRemoteAssesmentDescription</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_saRemoteAssesmentDescription</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_saRemoteAssesmentURL</t>
+  </si>
+  <si>
+    <t>SaRemoteAssesmentURL</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_saResults</t>
+  </si>
+  <si>
+    <t>SaResults</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_emailBodyAssesmentSchedule</t>
+  </si>
+  <si>
+    <t>EmailBodyAssesmentSchedule</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_emailSubjectAssementSchedule</t>
+  </si>
+  <si>
+    <t>EmailSubjectAssementSchedule</t>
+  </si>
+  <si>
+    <t>USNNewCandidates_EmailBodyHRResult</t>
+  </si>
+  <si>
+    <t>EmailBodyHRResult</t>
   </si>
 </sst>
 </file>
@@ -894,7 +984,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -937,6 +1027,9 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1813,7 +1906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -1978,8 +2071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2671,30 +2764,135 @@
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="74" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="75" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="76" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="77" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="78" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="79" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="80" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="73" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A73" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A74" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A75" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A76" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A77" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A78" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A79" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A80" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A81" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A82" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B82" s="32" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A83" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A84" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A85" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A86" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A87" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="89" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="90" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="91" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="92" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="93" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="94" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="95" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="96" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="97" ht="14.25" customHeight="1"/>
     <row r="98" ht="14.25" customHeight="1"/>
     <row r="99" ht="14.25" customHeight="1"/>
@@ -3589,6 +3787,6 @@
   </sheetData>
   <phoneticPr fontId="7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>